<commit_message>
Scriptie - Bijlage B afgemaakt + verder met Deelvraag 3 (TOC)
</commit_message>
<xml_diff>
--- a/Ploegen berekening.xlsx
+++ b/Ploegen berekening.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-60" windowWidth="25200" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
   <si>
     <t>Kg totaal matrix</t>
   </si>
@@ -76,13 +76,197 @@
   </si>
   <si>
     <t>is minuten per ploeg vermenigvuldigd met OEE percentage</t>
+  </si>
+  <si>
+    <t>stuks</t>
+  </si>
+  <si>
+    <t>feb</t>
+  </si>
+  <si>
+    <t>101RH 1</t>
+  </si>
+  <si>
+    <t>101RH 2</t>
+  </si>
+  <si>
+    <t>111BH 1</t>
+  </si>
+  <si>
+    <t>111BH 2</t>
+  </si>
+  <si>
+    <t>141BH</t>
+  </si>
+  <si>
+    <t>161CH</t>
+  </si>
+  <si>
+    <t>161RH</t>
+  </si>
+  <si>
+    <t>2KR 7</t>
+  </si>
+  <si>
+    <t>4KR 1</t>
+  </si>
+  <si>
+    <t>4KR 4</t>
+  </si>
+  <si>
+    <t>61RH 1</t>
+  </si>
+  <si>
+    <t>61RH 2</t>
+  </si>
+  <si>
+    <t>81BH 1</t>
+  </si>
+  <si>
+    <t>81RH 1</t>
+  </si>
+  <si>
+    <t>81RH 2</t>
+  </si>
+  <si>
+    <t>81RH 3</t>
+  </si>
+  <si>
+    <t>81RH 4</t>
+  </si>
+  <si>
+    <t>Lijn 1</t>
+  </si>
+  <si>
+    <t>Lijn 10</t>
+  </si>
+  <si>
+    <t>Lijn 11</t>
+  </si>
+  <si>
+    <t>Lijn 12</t>
+  </si>
+  <si>
+    <t>Lijn 13</t>
+  </si>
+  <si>
+    <t>Lijn 14</t>
+  </si>
+  <si>
+    <t>Lijn 2</t>
+  </si>
+  <si>
+    <t>Lijn 22</t>
+  </si>
+  <si>
+    <t>Lijn 23</t>
+  </si>
+  <si>
+    <t>Lijn 24</t>
+  </si>
+  <si>
+    <t>Lijn 25</t>
+  </si>
+  <si>
+    <t>Lijn 26</t>
+  </si>
+  <si>
+    <t>Lijn 27</t>
+  </si>
+  <si>
+    <t>Lijn 28</t>
+  </si>
+  <si>
+    <t>Lijn 29</t>
+  </si>
+  <si>
+    <t>Lijn 3</t>
+  </si>
+  <si>
+    <t>Lijn 30</t>
+  </si>
+  <si>
+    <t>Lijn 31</t>
+  </si>
+  <si>
+    <t>Lijn 4</t>
+  </si>
+  <si>
+    <t>Lijn 5</t>
+  </si>
+  <si>
+    <t>Lijn 6</t>
+  </si>
+  <si>
+    <t>Lijn 7</t>
+  </si>
+  <si>
+    <t>Lijn 8</t>
+  </si>
+  <si>
+    <t>Lijn 9</t>
+  </si>
+  <si>
+    <t>Oven 1</t>
+  </si>
+  <si>
+    <t>Oven 2</t>
+  </si>
+  <si>
+    <t>Oven 3</t>
+  </si>
+  <si>
+    <t>SUM(Productie) (stuks)</t>
+  </si>
+  <si>
+    <t>Naam</t>
+  </si>
+  <si>
+    <t>AVG(Gewicht) (kg)</t>
+  </si>
+  <si>
+    <t>AVG(OEE) (fractal (0-1))</t>
+  </si>
+  <si>
+    <t>AVG(LijnSnelheid) (stuks/min)</t>
+  </si>
+  <si>
+    <t>Ploegen na</t>
+  </si>
+  <si>
+    <t>Ploegen voor</t>
+  </si>
+  <si>
+    <t>Buffer na (stuks)</t>
+  </si>
+  <si>
+    <t>Buffer voor (stuks)</t>
+  </si>
+  <si>
+    <t>SLIJPERIJ Productie</t>
+  </si>
+  <si>
+    <t>Werkelijkheid</t>
+  </si>
+  <si>
+    <t>Simulatie</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="172" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="174" formatCode="0.00000000000000000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +275,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,6 +351,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -174,6 +367,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -564,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,10 +773,17 @@
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -590,54 +795,54 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="17"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="18">
+      <c r="B4" s="19">
         <f>1699000*0.005</f>
         <v>8495</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="16">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="17">
         <f>B4/(B6*D6*F6*H6)</f>
         <v>18.05909863945578</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
     </row>
     <row r="5" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -648,11 +853,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
@@ -677,11 +882,11 @@
       <c r="H6" s="8">
         <v>0.7</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
     </row>
     <row r="7" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -780,7 +985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B15*B16</f>
         <v>336</v>
@@ -792,7 +997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <f>B14/B17</f>
         <v>18.059098639455783</v>
@@ -800,6 +1005,1183 @@
       <c r="D18" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D20" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <f>SUM(E42:E65)</f>
+        <v>95907961</v>
+      </c>
+      <c r="E21">
+        <v>88164000</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="E22">
+        <f>E21/D21*100</f>
+        <v>91.925632742833514</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D24" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <v>5762552</v>
+      </c>
+      <c r="F25">
+        <v>1000</v>
+      </c>
+      <c r="G25">
+        <v>1000</v>
+      </c>
+      <c r="H25" s="25">
+        <f>8.95748870850083/1000</f>
+        <v>8.9574887085008287E-3</v>
+      </c>
+      <c r="J25" s="24">
+        <v>393.99999618530302</v>
+      </c>
+      <c r="L25" s="23">
+        <v>0.56569849196975597</v>
+      </c>
+      <c r="M25" s="9">
+        <f>F25*H25/(J25*H25*480*L25)</f>
+        <v>9.3471136663787879E-3</v>
+      </c>
+      <c r="N25" s="9">
+        <f>G25*H25/(J25*H25*480*L25)</f>
+        <v>9.3471136663787879E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26">
+        <v>7839660</v>
+      </c>
+      <c r="F26">
+        <v>1000</v>
+      </c>
+      <c r="G26">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="25">
+        <f>6.90730498504868/1000</f>
+        <v>6.9073049850486802E-3</v>
+      </c>
+      <c r="J26" s="24">
+        <v>403.00000190734897</v>
+      </c>
+      <c r="L26" s="23">
+        <v>0.69312423221654296</v>
+      </c>
+      <c r="M26" s="9">
+        <f>F26*H26/(J26*H26*480*L26)</f>
+        <v>7.4583478061009106E-3</v>
+      </c>
+      <c r="N26" s="9">
+        <f t="shared" ref="N26:N41" si="0">G26*H26/(J26*H26*480*L26)</f>
+        <v>7.4583478061009106E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27">
+        <v>8029520</v>
+      </c>
+      <c r="F27">
+        <v>3297000</v>
+      </c>
+      <c r="G27">
+        <v>1000</v>
+      </c>
+      <c r="H27" s="25">
+        <f>3.08246622711922/1000</f>
+        <v>3.08246622711922E-3</v>
+      </c>
+      <c r="J27" s="24">
+        <v>427.99999237060501</v>
+      </c>
+      <c r="L27" s="23">
+        <v>0.68487961598823399</v>
+      </c>
+      <c r="M27" s="9">
+        <f>F27*H27/(J27*H27*480*L27)</f>
+        <v>23.432558393973533</v>
+      </c>
+      <c r="N27" s="9">
+        <f t="shared" si="0"/>
+        <v>7.1072363948964309E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28">
+        <v>9788896</v>
+      </c>
+      <c r="F28">
+        <v>3268000</v>
+      </c>
+      <c r="G28">
+        <v>4000</v>
+      </c>
+      <c r="H28" s="25">
+        <f>3.47811007659957/1000</f>
+        <v>3.47811007659957E-3</v>
+      </c>
+      <c r="J28" s="24">
+        <v>423.00001144409202</v>
+      </c>
+      <c r="L28" s="23">
+        <v>0.834458335873144</v>
+      </c>
+      <c r="M28" s="9">
+        <f>F28*H28/(J28*H28*480*L28)</f>
+        <v>19.288380908226056</v>
+      </c>
+      <c r="N28" s="9">
+        <f t="shared" si="0"/>
+        <v>2.3608789361353803E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>7846772</v>
+      </c>
+      <c r="F29">
+        <v>40000</v>
+      </c>
+      <c r="G29">
+        <v>1000</v>
+      </c>
+      <c r="H29" s="25">
+        <f>6.30362333829065/1000</f>
+        <v>6.3036233382906494E-3</v>
+      </c>
+      <c r="J29" s="24">
+        <v>341.99998855590798</v>
+      </c>
+      <c r="L29" s="23">
+        <v>0.77551487700821398</v>
+      </c>
+      <c r="M29" s="9">
+        <f>F29*H29/(J29*H29*480*L29)</f>
+        <v>0.31419735807327243</v>
+      </c>
+      <c r="N29" s="9">
+        <f t="shared" si="0"/>
+        <v>7.854933951831811E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30">
+        <v>4519512</v>
+      </c>
+      <c r="F30">
+        <v>1000</v>
+      </c>
+      <c r="G30">
+        <v>1000</v>
+      </c>
+      <c r="H30" s="25">
+        <f>20.9671261909317/1000</f>
+        <v>2.09671261909317E-2</v>
+      </c>
+      <c r="J30" s="24">
+        <v>266.99998855590798</v>
+      </c>
+      <c r="L30" s="23">
+        <v>0.60117790539627902</v>
+      </c>
+      <c r="M30" s="9">
+        <f>F30*H30/(J30*H30*480*L30)</f>
+        <v>1.2979097919587866E-2</v>
+      </c>
+      <c r="N30" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2979097919587866E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31">
+        <v>3501620</v>
+      </c>
+      <c r="F31">
+        <v>29000</v>
+      </c>
+      <c r="G31">
+        <v>1000</v>
+      </c>
+      <c r="H31" s="25">
+        <f>21.8599834611596/1000</f>
+        <v>2.18599834611596E-2</v>
+      </c>
+      <c r="J31" s="24">
+        <v>261.402118661305</v>
+      </c>
+      <c r="L31" s="23">
+        <v>0.418486626636843</v>
+      </c>
+      <c r="M31" s="9">
+        <f>F31*H31/(J31*H31*480*L31)</f>
+        <v>0.55228859289172139</v>
+      </c>
+      <c r="N31" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9044434237645565E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <v>1482347</v>
+      </c>
+      <c r="F32">
+        <v>1000</v>
+      </c>
+      <c r="G32">
+        <v>1000</v>
+      </c>
+      <c r="H32" s="25">
+        <f>3.26560463104033/1000</f>
+        <v>3.2656046310403299E-3</v>
+      </c>
+      <c r="J32" s="24">
+        <v>210</v>
+      </c>
+      <c r="L32" s="23">
+        <v>0.90586364273396902</v>
+      </c>
+      <c r="M32" s="9">
+        <f>F32*H32/(J32*H32*480*L32)</f>
+        <v>1.0951576432291344E-2</v>
+      </c>
+      <c r="N32" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0951576432291344E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33">
+        <v>585382</v>
+      </c>
+      <c r="F33">
+        <v>1000</v>
+      </c>
+      <c r="G33">
+        <v>1000</v>
+      </c>
+      <c r="H33" s="25">
+        <f>4.0533018791114/1000</f>
+        <v>4.0533018791113996E-3</v>
+      </c>
+      <c r="J33" s="24">
+        <v>165</v>
+      </c>
+      <c r="L33" s="23">
+        <v>0.87108941796671102</v>
+      </c>
+      <c r="M33" s="9">
+        <f>F33*H33/(J33*H33*480*L33)</f>
+        <v>1.4494795098917325E-2</v>
+      </c>
+      <c r="N33" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4494795098917325E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34">
+        <v>1074539</v>
+      </c>
+      <c r="F34">
+        <v>1000</v>
+      </c>
+      <c r="G34">
+        <v>1000</v>
+      </c>
+      <c r="H34" s="25">
+        <f>19.4119963157937/1000</f>
+        <v>1.9411996315793701E-2</v>
+      </c>
+      <c r="J34" s="24">
+        <v>165</v>
+      </c>
+      <c r="L34" s="23">
+        <v>0.95861700118005799</v>
+      </c>
+      <c r="M34" s="9">
+        <f>F34*H34/(J34*H34*480*L34)</f>
+        <v>1.3171331836092716E-2</v>
+      </c>
+      <c r="N34" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3171331836092716E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35">
+        <v>12187040</v>
+      </c>
+      <c r="F35">
+        <v>2293000</v>
+      </c>
+      <c r="G35">
+        <v>1000</v>
+      </c>
+      <c r="H35" s="25">
+        <f>1.92200832952954/1000</f>
+        <v>1.9220083295295399E-3</v>
+      </c>
+      <c r="J35" s="24">
+        <v>625.00001907348599</v>
+      </c>
+      <c r="L35" s="23">
+        <v>0.72786778963234999</v>
+      </c>
+      <c r="M35" s="9">
+        <f>F35*H35/(J35*H35*480*L35)</f>
+        <v>10.500990988951457</v>
+      </c>
+      <c r="N35" s="9">
+        <f t="shared" si="0"/>
+        <v>4.579586126886811E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36">
+        <v>12407600</v>
+      </c>
+      <c r="F36">
+        <v>3671000</v>
+      </c>
+      <c r="G36">
+        <v>1000</v>
+      </c>
+      <c r="H36" s="25">
+        <f>2.15905238196507/1000</f>
+        <v>2.1590523819650701E-3</v>
+      </c>
+      <c r="J36" s="24">
+        <v>660</v>
+      </c>
+      <c r="L36" s="23">
+        <v>0.69721304997938505</v>
+      </c>
+      <c r="M36" s="9">
+        <f>F36*H36/(J36*H36*480*L36)</f>
+        <v>16.620102744197272</v>
+      </c>
+      <c r="N36" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5274047246519396E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37">
+        <v>15327560</v>
+      </c>
+      <c r="F37">
+        <v>55000</v>
+      </c>
+      <c r="G37">
+        <v>1000</v>
+      </c>
+      <c r="H37" s="25">
+        <f>0.66846345040472/1000</f>
+        <v>6.6846345040472003E-4</v>
+      </c>
+      <c r="J37" s="24">
+        <v>633.826975537767</v>
+      </c>
+      <c r="L37" s="23">
+        <v>0.82250949258375305</v>
+      </c>
+      <c r="M37" s="9">
+        <f>F37*H37/(J37*H37*480*L37)</f>
+        <v>0.21979095424129719</v>
+      </c>
+      <c r="N37" s="9">
+        <f t="shared" si="0"/>
+        <v>3.9961991680235853E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38">
+        <v>10384816</v>
+      </c>
+      <c r="F38">
+        <v>1000</v>
+      </c>
+      <c r="G38">
+        <v>1000</v>
+      </c>
+      <c r="H38" s="25">
+        <f>4.45269698507593/1000</f>
+        <v>4.4526969850759296E-3</v>
+      </c>
+      <c r="J38" s="24">
+        <v>479.17350733281802</v>
+      </c>
+      <c r="L38" s="23">
+        <v>0.74978989337439095</v>
+      </c>
+      <c r="M38" s="9">
+        <f>F38*H38/(J38*H38*480*L38)</f>
+        <v>5.7986431344907319E-3</v>
+      </c>
+      <c r="N38" s="9">
+        <f t="shared" si="0"/>
+        <v>5.7986431344907319E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39">
+        <v>13252760</v>
+      </c>
+      <c r="F39">
+        <v>1000</v>
+      </c>
+      <c r="G39">
+        <v>1000</v>
+      </c>
+      <c r="H39" s="25">
+        <f>3.69815107657532/1000</f>
+        <v>3.6981510765753201E-3</v>
+      </c>
+      <c r="J39" s="24">
+        <v>483.00001144409202</v>
+      </c>
+      <c r="L39" s="23">
+        <v>0.891981577941797</v>
+      </c>
+      <c r="M39" s="9">
+        <f>F39*H39/(J39*H39*480*L39)</f>
+        <v>4.8356597660512181E-3</v>
+      </c>
+      <c r="N39" s="9">
+        <f t="shared" si="0"/>
+        <v>4.8356597660512181E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40">
+        <v>12088104</v>
+      </c>
+      <c r="F40">
+        <v>2507000</v>
+      </c>
+      <c r="G40">
+        <v>1000</v>
+      </c>
+      <c r="H40" s="25">
+        <f>3.89941847511468/1000</f>
+        <v>3.8994184751146798E-3</v>
+      </c>
+      <c r="J40" s="24">
+        <v>483.00001144409202</v>
+      </c>
+      <c r="L40" s="23">
+        <v>0.83073242756994803</v>
+      </c>
+      <c r="M40" s="9">
+        <f>F40*H40/(J40*H40*480*L40)</f>
+        <v>13.01681678529294</v>
+      </c>
+      <c r="N40" s="9">
+        <f t="shared" si="0"/>
+        <v>5.1921885860761628E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41">
+        <v>10638560</v>
+      </c>
+      <c r="F41">
+        <v>1000</v>
+      </c>
+      <c r="G41">
+        <v>1000</v>
+      </c>
+      <c r="H41" s="25">
+        <f>3.78381132159395/1000</f>
+        <v>3.78381132159395E-3</v>
+      </c>
+      <c r="J41" s="24">
+        <v>489.17941116760102</v>
+      </c>
+      <c r="L41" s="23">
+        <v>0.67623798704798499</v>
+      </c>
+      <c r="M41" s="9">
+        <f>F41*H41/(J41*H41*480*L41)</f>
+        <v>6.2978313937329848E-3</v>
+      </c>
+      <c r="N41" s="9">
+        <f>G41*H41/(J41*H41*480*L41)</f>
+        <v>6.2978313937329848E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42">
+        <v>4502244</v>
+      </c>
+      <c r="H42" s="25">
+        <f>1.79833904216144/1000</f>
+        <v>1.7983390421614401E-3</v>
+      </c>
+      <c r="J42" s="24">
+        <v>292.09190942222602</v>
+      </c>
+      <c r="L42" s="23">
+        <v>0.48793678480548203</v>
+      </c>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+    </row>
+    <row r="43" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43">
+        <v>4605108</v>
+      </c>
+      <c r="H43" s="25">
+        <f>3.99685466418631/1000</f>
+        <v>3.9968546641863095E-3</v>
+      </c>
+      <c r="J43" s="24">
+        <v>286.41874550067899</v>
+      </c>
+      <c r="L43" s="23">
+        <v>0.57933407298994299</v>
+      </c>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+    </row>
+    <row r="44" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44">
+        <v>4888464</v>
+      </c>
+      <c r="H44" s="25">
+        <f>2.98636386831565/1000</f>
+        <v>2.98636386831565E-3</v>
+      </c>
+      <c r="J44" s="24">
+        <v>300</v>
+      </c>
+      <c r="L44" s="23">
+        <v>0.64726151267721199</v>
+      </c>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+    </row>
+    <row r="45" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45">
+        <v>5565444</v>
+      </c>
+      <c r="H45" s="25">
+        <f>2.85934264011567/1000</f>
+        <v>2.8593426401156701E-3</v>
+      </c>
+      <c r="J45" s="24">
+        <v>312.85597082724303</v>
+      </c>
+      <c r="L45" s="23">
+        <v>0.66834057024015203</v>
+      </c>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+    </row>
+    <row r="46" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46">
+        <v>3931000</v>
+      </c>
+      <c r="H46" s="25">
+        <f>4.00765759075619/1000</f>
+        <v>4.00765759075619E-3</v>
+      </c>
+      <c r="J46" s="24">
+        <v>263.16579583595001</v>
+      </c>
+      <c r="L46" s="23">
+        <v>0.49372229488084601</v>
+      </c>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+    </row>
+    <row r="47" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47">
+        <v>4196322</v>
+      </c>
+      <c r="H47" s="25">
+        <f>4.37136935664059/1000</f>
+        <v>4.3713693566405894E-3</v>
+      </c>
+      <c r="J47" s="24">
+        <v>279.99999046325701</v>
+      </c>
+      <c r="L47" s="23">
+        <v>0.57930844113381696</v>
+      </c>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+    </row>
+    <row r="48" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48">
+        <v>5157352</v>
+      </c>
+      <c r="H48" s="25">
+        <f>3.1836603956552/1000</f>
+        <v>3.1836603956552001E-3</v>
+      </c>
+      <c r="J48" s="24">
+        <v>284.72995178137899</v>
+      </c>
+      <c r="L48" s="23">
+        <v>0.66998113108977297</v>
+      </c>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+    </row>
+    <row r="49" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>45</v>
+      </c>
+      <c r="E49">
+        <v>2632713</v>
+      </c>
+      <c r="H49" s="25">
+        <f>8.93216269229009/1000</f>
+        <v>8.9321626922900903E-3</v>
+      </c>
+      <c r="J49" s="24">
+        <v>150.50029379138101</v>
+      </c>
+      <c r="L49" s="23">
+        <v>0.68915148180501296</v>
+      </c>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+    </row>
+    <row r="50" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50">
+        <v>2005412</v>
+      </c>
+      <c r="H50" s="25">
+        <f>10.1964611046349/1000</f>
+        <v>1.0196461104634898E-2</v>
+      </c>
+      <c r="J50" s="24">
+        <v>146.40475074882301</v>
+      </c>
+      <c r="L50" s="23">
+        <v>0.52990503974713299</v>
+      </c>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+    </row>
+    <row r="51" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E51">
+        <v>7251312</v>
+      </c>
+      <c r="H51" s="25">
+        <f>2.33542107577583/1000</f>
+        <v>2.3354210757758299E-3</v>
+      </c>
+      <c r="J51" s="24">
+        <v>279.99999046325701</v>
+      </c>
+      <c r="L51" s="23">
+        <v>0.75486486993963497</v>
+      </c>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+    </row>
+    <row r="52" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52">
+        <v>6086916</v>
+      </c>
+      <c r="H52" s="25">
+        <f>3.24181305143847/1000</f>
+        <v>3.2418130514384699E-3</v>
+      </c>
+      <c r="J52" s="24">
+        <v>274.87825511216801</v>
+      </c>
+      <c r="L52" s="23">
+        <v>0.68936781111033496</v>
+      </c>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+    </row>
+    <row r="53" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53">
+        <v>4209796</v>
+      </c>
+      <c r="H53" s="25">
+        <f>1.8650088585347/1000</f>
+        <v>1.8650088585347E-3</v>
+      </c>
+      <c r="J53" s="24">
+        <v>264.09920060626303</v>
+      </c>
+      <c r="L53" s="23">
+        <v>0.54235818587372897</v>
+      </c>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+    </row>
+    <row r="54" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54">
+        <v>4605340</v>
+      </c>
+      <c r="H54" s="25">
+        <f>2.04443472676232/1000</f>
+        <v>2.04443472676232E-3</v>
+      </c>
+      <c r="J54" s="24">
+        <v>284.73175807738698</v>
+      </c>
+      <c r="L54" s="23">
+        <v>0.56223781896990799</v>
+      </c>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+    </row>
+    <row r="55" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55">
+        <v>4438288</v>
+      </c>
+      <c r="H55" s="25">
+        <f>4.90999985408869/1000</f>
+        <v>4.9099998540886904E-3</v>
+      </c>
+      <c r="J55" s="24">
+        <v>260.00000953674299</v>
+      </c>
+      <c r="L55" s="23">
+        <v>0.56317894721065598</v>
+      </c>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+    </row>
+    <row r="56" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56">
+        <v>1520167</v>
+      </c>
+      <c r="H56" s="25">
+        <f>25.8720012610716/1000</f>
+        <v>2.58720012610716E-2</v>
+      </c>
+      <c r="J56" s="24">
+        <v>92.830658335881296</v>
+      </c>
+      <c r="L56" s="23">
+        <v>0.55287646564834803</v>
+      </c>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+    </row>
+    <row r="57" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57">
+        <v>3040836</v>
+      </c>
+      <c r="H57" s="25">
+        <f>3.92250190209233/1000</f>
+        <v>3.9225019020923298E-3</v>
+      </c>
+      <c r="J57" s="24">
+        <v>299.84565678211101</v>
+      </c>
+      <c r="L57" s="23">
+        <v>0.62207607852207103</v>
+      </c>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+    </row>
+    <row r="58" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58">
+        <v>914952</v>
+      </c>
+      <c r="H58" s="25">
+        <f>26.1312100197428/1000</f>
+        <v>2.61312100197428E-2</v>
+      </c>
+      <c r="J58" s="24">
+        <v>87.513553970476096</v>
+      </c>
+      <c r="L58" s="23">
+        <v>0.31301547333277502</v>
+      </c>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+    </row>
+    <row r="59" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59">
+        <v>619432</v>
+      </c>
+      <c r="H59" s="25">
+        <f>62.3202702976991/1000</f>
+        <v>6.2320270297699105E-2</v>
+      </c>
+      <c r="J59" s="24">
+        <v>60.480449534168301</v>
+      </c>
+      <c r="L59" s="23">
+        <v>0.41502337592158201</v>
+      </c>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+    </row>
+    <row r="60" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60">
+        <v>5507668</v>
+      </c>
+      <c r="H60" s="25">
+        <f>4.99769163699139/1000</f>
+        <v>4.9976916369913896E-3</v>
+      </c>
+      <c r="J60" s="24">
+        <v>279.99999046325701</v>
+      </c>
+      <c r="L60" s="23">
+        <v>0.67152074294702602</v>
+      </c>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+    </row>
+    <row r="61" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>57</v>
+      </c>
+      <c r="E61">
+        <v>6828400</v>
+      </c>
+      <c r="H61" s="25">
+        <f>4.68241980228823/1000</f>
+        <v>4.6824198022882299E-3</v>
+      </c>
+      <c r="J61" s="24">
+        <v>260.00000953674299</v>
+      </c>
+      <c r="L61" s="23">
+        <v>0.73077789643872104</v>
+      </c>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+    </row>
+    <row r="62" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62">
+        <v>5567112</v>
+      </c>
+      <c r="H62" s="25">
+        <f>3.95233314877769/1000</f>
+        <v>3.9523331487776904E-3</v>
+      </c>
+      <c r="J62" s="24">
+        <v>277.82067109152899</v>
+      </c>
+      <c r="L62" s="23">
+        <v>0.62285858762021695</v>
+      </c>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+    </row>
+    <row r="63" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63">
+        <v>3268978</v>
+      </c>
+      <c r="H63" s="25">
+        <f>6.93669468434003/1000</f>
+        <v>6.9366946843400301E-3</v>
+      </c>
+      <c r="J63" s="24">
+        <v>176.52903509502201</v>
+      </c>
+      <c r="L63" s="23">
+        <v>0.59053560942063699</v>
+      </c>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+    </row>
+    <row r="64" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64">
+        <v>2206532</v>
+      </c>
+      <c r="H64" s="25">
+        <f>15.5647624267794/1000</f>
+        <v>1.5564762426779399E-2</v>
+      </c>
+      <c r="J64" s="24">
+        <v>97.6573178133619</v>
+      </c>
+      <c r="L64" s="23">
+        <v>0.75032931483717602</v>
+      </c>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+    </row>
+    <row r="65" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>61</v>
+      </c>
+      <c r="E65">
+        <v>2358173</v>
+      </c>
+      <c r="H65" s="25">
+        <f>21.7001264386141/1000</f>
+        <v>2.17001264386141E-2</v>
+      </c>
+      <c r="J65" s="24">
+        <v>98.674181058758094</v>
+      </c>
+      <c r="L65" s="23">
+        <v>0.74878745231924404</v>
+      </c>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+    </row>
+    <row r="66" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" s="21">
+        <f>114985.40625/H66</f>
+        <v>34246634.877882801</v>
+      </c>
+      <c r="F66">
+        <v>7523000</v>
+      </c>
+      <c r="H66" s="25">
+        <f>3.35756802558899/1000</f>
+        <v>3.3575680255889901E-3</v>
+      </c>
+      <c r="J66" s="24">
+        <f>2.57500000298023*(500/H66)</f>
+        <v>383462.07483443606</v>
+      </c>
+      <c r="L66" s="23">
+        <v>1.1790338355157499</v>
+      </c>
+      <c r="M66" s="9">
+        <f>F66*H66/(J66*H66*480*L66)</f>
+        <v>3.4665792898722972E-2</v>
+      </c>
+      <c r="N66" s="9"/>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" s="22">
+        <f>90653.4375/H67</f>
+        <v>1711510.3729148097</v>
+      </c>
+      <c r="F67">
+        <v>57000</v>
+      </c>
+      <c r="H67" s="25">
+        <f>52.9669226284685/1000</f>
+        <v>5.2966922628468499E-2</v>
+      </c>
+      <c r="J67" s="24">
+        <f>3.29999998211861*(500/H67)</f>
+        <v>31151.517006813381</v>
+      </c>
+      <c r="L67" s="23">
+        <v>0.75279795798154303</v>
+      </c>
+      <c r="M67" s="9">
+        <f>F67*H67/(J67*H67*480*L67)</f>
+        <v>5.0637934803451114E-3</v>
+      </c>
+      <c r="N67" s="9"/>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="21">
+        <f>108075.75/H68</f>
+        <v>31899571.911138851</v>
+      </c>
+      <c r="F68">
+        <v>7523000</v>
+      </c>
+      <c r="H68" s="25">
+        <f>3.38800001144409/1000</f>
+        <v>3.38800001144409E-3</v>
+      </c>
+      <c r="J68" s="24">
+        <f>3.87096762657166*(500/H68)</f>
+        <v>571276.2121452461</v>
+      </c>
+      <c r="L68" s="23">
+        <v>0.76389627203334698</v>
+      </c>
+      <c r="M68" s="9">
+        <f>F68*H68/(J68*H68*480*L68)</f>
+        <v>3.5914456070995963E-2</v>
+      </c>
+      <c r="N68" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -813,6 +2195,18 @@
     <mergeCell ref="I4:I6"/>
     <mergeCell ref="J2:K2"/>
   </mergeCells>
+  <conditionalFormatting sqref="L25:L68">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0.4"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="num" val="0.85"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFC000"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Scriptie - Deelvraag 4 (Experimenten) - verder gewerkt
</commit_message>
<xml_diff>
--- a/Ploegen berekening.xlsx
+++ b/Ploegen berekening.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Kg totaal matrix</t>
   </si>
@@ -253,6 +253,21 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Gem. ploegen na persen</t>
+  </si>
+  <si>
+    <t>AVG(AVG(Gewicht)) kg</t>
+  </si>
+  <si>
+    <t>AVG(AVG(LijnSnelheid)) (stuks/min)</t>
+  </si>
+  <si>
+    <t>AVG(AVG(OEE)) (fractal (0-1))</t>
+  </si>
+  <si>
+    <t>AVG(Ploegen na)</t>
   </si>
 </sst>
 </file>
@@ -262,9 +277,9 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
-    <numFmt numFmtId="172" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="173" formatCode="0.0000000000000000"/>
-    <numFmt numFmtId="174" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000000000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -352,6 +367,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,11 +387,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -410,7 +425,7 @@
         <xdr:cNvPr id="2" name="Equals 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{81193C8A-C1C1-4CDE-AFB3-EDEEA4AEF6F1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81193C8A-C1C1-4CDE-AFB3-EDEEA4AEF6F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -754,7 +769,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -762,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
+      <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,12 +791,13 @@
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -795,54 +811,54 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="18"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="19">
+      <c r="B4" s="24">
         <f>1699000*0.005</f>
         <v>8495</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="17">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="22">
         <f>B4/(B6*D6*F6*H6)</f>
         <v>18.05909863945578</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -853,11 +869,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
@@ -882,11 +898,11 @@
       <c r="H6" s="8">
         <v>0.7</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -1026,22 +1042,30 @@
         <v>95907961</v>
       </c>
       <c r="E21">
-        <v>88164000</v>
+        <v>88181000</v>
       </c>
       <c r="F21" t="s">
         <v>19</v>
       </c>
+      <c r="M21" s="15" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D22">
+        <f>D21/D21*100</f>
         <v>100</v>
       </c>
       <c r="E22">
-        <f>E21/D21*100</f>
-        <v>91.925632742833514</v>
+        <f>E21/D21*D22</f>
+        <v>91.943358070139766</v>
       </c>
       <c r="F22" t="s">
         <v>77</v>
+      </c>
+      <c r="M22" s="9">
+        <f>AVERAGE(M25:M41)</f>
+        <v>4.0433706699256398</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -1088,18 +1112,18 @@
       <c r="G25">
         <v>1000</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="20">
         <f>8.95748870850083/1000</f>
         <v>8.9574887085008287E-3</v>
       </c>
-      <c r="J25" s="24">
+      <c r="J25" s="19">
         <v>393.99999618530302</v>
       </c>
-      <c r="L25" s="23">
+      <c r="L25" s="18">
         <v>0.56569849196975597</v>
       </c>
       <c r="M25" s="9">
-        <f>F25*H25/(J25*H25*480*L25)</f>
+        <f t="shared" ref="M25:M41" si="0">F25*H25/(J25*H25*480*L25)</f>
         <v>9.3471136663787879E-3</v>
       </c>
       <c r="N25" s="9">
@@ -1120,22 +1144,22 @@
       <c r="G26">
         <v>1000</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="20">
         <f>6.90730498504868/1000</f>
         <v>6.9073049850486802E-3</v>
       </c>
-      <c r="J26" s="24">
+      <c r="J26" s="19">
         <v>403.00000190734897</v>
       </c>
-      <c r="L26" s="23">
+      <c r="L26" s="18">
         <v>0.69312423221654296</v>
       </c>
       <c r="M26" s="9">
-        <f>F26*H26/(J26*H26*480*L26)</f>
+        <f t="shared" si="0"/>
         <v>7.4583478061009106E-3</v>
       </c>
       <c r="N26" s="9">
-        <f t="shared" ref="N26:N41" si="0">G26*H26/(J26*H26*480*L26)</f>
+        <f t="shared" ref="N26:N40" si="1">G26*H26/(J26*H26*480*L26)</f>
         <v>7.4583478061009106E-3</v>
       </c>
     </row>
@@ -1147,27 +1171,27 @@
         <v>8029520</v>
       </c>
       <c r="F27">
-        <v>3297000</v>
+        <v>2590000</v>
       </c>
       <c r="G27">
         <v>1000</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="20">
         <f>3.08246622711922/1000</f>
         <v>3.08246622711922E-3</v>
       </c>
-      <c r="J27" s="24">
+      <c r="J27" s="19">
         <v>427.99999237060501</v>
       </c>
-      <c r="L27" s="23">
+      <c r="L27" s="18">
         <v>0.68487961598823399</v>
       </c>
       <c r="M27" s="9">
-        <f>F27*H27/(J27*H27*480*L27)</f>
-        <v>23.432558393973533</v>
+        <f t="shared" si="0"/>
+        <v>18.407742262781756</v>
       </c>
       <c r="N27" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1072363948964309E-3</v>
       </c>
     </row>
@@ -1179,27 +1203,27 @@
         <v>9788896</v>
       </c>
       <c r="F28">
-        <v>3268000</v>
+        <v>2653000</v>
       </c>
       <c r="G28">
         <v>4000</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="20">
         <f>3.47811007659957/1000</f>
         <v>3.47811007659957E-3</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J28" s="19">
         <v>423.00001144409202</v>
       </c>
-      <c r="L28" s="23">
+      <c r="L28" s="18">
         <v>0.834458335873144</v>
       </c>
       <c r="M28" s="9">
         <f>F28*H28/(J28*H28*480*L28)</f>
-        <v>19.288380908226056</v>
+        <v>15.65852954391791</v>
       </c>
       <c r="N28" s="9">
-        <f t="shared" si="0"/>
+        <f>G28*H28/(J28*H28*480*L28)</f>
         <v>2.3608789361353803E-2</v>
       </c>
     </row>
@@ -1216,22 +1240,22 @@
       <c r="G29">
         <v>1000</v>
       </c>
-      <c r="H29" s="25">
+      <c r="H29" s="20">
         <f>6.30362333829065/1000</f>
         <v>6.3036233382906494E-3</v>
       </c>
-      <c r="J29" s="24">
+      <c r="J29" s="19">
         <v>341.99998855590798</v>
       </c>
-      <c r="L29" s="23">
+      <c r="L29" s="18">
         <v>0.77551487700821398</v>
       </c>
       <c r="M29" s="9">
-        <f>F29*H29/(J29*H29*480*L29)</f>
+        <f t="shared" si="0"/>
         <v>0.31419735807327243</v>
       </c>
       <c r="N29" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.854933951831811E-3</v>
       </c>
     </row>
@@ -1248,22 +1272,22 @@
       <c r="G30">
         <v>1000</v>
       </c>
-      <c r="H30" s="25">
+      <c r="H30" s="20">
         <f>20.9671261909317/1000</f>
         <v>2.09671261909317E-2</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="19">
         <v>266.99998855590798</v>
       </c>
-      <c r="L30" s="23">
+      <c r="L30" s="18">
         <v>0.60117790539627902</v>
       </c>
       <c r="M30" s="9">
-        <f>F30*H30/(J30*H30*480*L30)</f>
+        <f t="shared" si="0"/>
         <v>1.2979097919587866E-2</v>
       </c>
       <c r="N30" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2979097919587866E-2</v>
       </c>
     </row>
@@ -1280,22 +1304,22 @@
       <c r="G31">
         <v>1000</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="20">
         <f>21.8599834611596/1000</f>
         <v>2.18599834611596E-2</v>
       </c>
-      <c r="J31" s="24">
+      <c r="J31" s="19">
         <v>261.402118661305</v>
       </c>
-      <c r="L31" s="23">
+      <c r="L31" s="18">
         <v>0.418486626636843</v>
       </c>
       <c r="M31" s="9">
-        <f>F31*H31/(J31*H31*480*L31)</f>
+        <f t="shared" si="0"/>
         <v>0.55228859289172139</v>
       </c>
       <c r="N31" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9044434237645565E-2</v>
       </c>
     </row>
@@ -1312,22 +1336,22 @@
       <c r="G32">
         <v>1000</v>
       </c>
-      <c r="H32" s="25">
+      <c r="H32" s="20">
         <f>3.26560463104033/1000</f>
         <v>3.2656046310403299E-3</v>
       </c>
-      <c r="J32" s="24">
+      <c r="J32" s="19">
         <v>210</v>
       </c>
-      <c r="L32" s="23">
+      <c r="L32" s="18">
         <v>0.90586364273396902</v>
       </c>
       <c r="M32" s="9">
-        <f>F32*H32/(J32*H32*480*L32)</f>
+        <f t="shared" si="0"/>
         <v>1.0951576432291344E-2</v>
       </c>
       <c r="N32" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0951576432291344E-2</v>
       </c>
     </row>
@@ -1344,22 +1368,22 @@
       <c r="G33">
         <v>1000</v>
       </c>
-      <c r="H33" s="25">
+      <c r="H33" s="20">
         <f>4.0533018791114/1000</f>
         <v>4.0533018791113996E-3</v>
       </c>
-      <c r="J33" s="24">
+      <c r="J33" s="19">
         <v>165</v>
       </c>
-      <c r="L33" s="23">
+      <c r="L33" s="18">
         <v>0.87108941796671102</v>
       </c>
       <c r="M33" s="9">
-        <f>F33*H33/(J33*H33*480*L33)</f>
+        <f t="shared" si="0"/>
         <v>1.4494795098917325E-2</v>
       </c>
       <c r="N33" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4494795098917325E-2</v>
       </c>
     </row>
@@ -1376,22 +1400,22 @@
       <c r="G34">
         <v>1000</v>
       </c>
-      <c r="H34" s="25">
+      <c r="H34" s="20">
         <f>19.4119963157937/1000</f>
         <v>1.9411996315793701E-2</v>
       </c>
-      <c r="J34" s="24">
+      <c r="J34" s="19">
         <v>165</v>
       </c>
-      <c r="L34" s="23">
+      <c r="L34" s="18">
         <v>0.95861700118005799</v>
       </c>
       <c r="M34" s="9">
-        <f>F34*H34/(J34*H34*480*L34)</f>
+        <f t="shared" si="0"/>
         <v>1.3171331836092716E-2</v>
       </c>
       <c r="N34" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3171331836092716E-2</v>
       </c>
     </row>
@@ -1403,27 +1427,27 @@
         <v>12187040</v>
       </c>
       <c r="F35">
-        <v>2293000</v>
+        <v>2181000</v>
       </c>
       <c r="G35">
         <v>1000</v>
       </c>
-      <c r="H35" s="25">
+      <c r="H35" s="20">
         <f>1.92200832952954/1000</f>
         <v>1.9220083295295399E-3</v>
       </c>
-      <c r="J35" s="24">
+      <c r="J35" s="19">
         <v>625.00001907348599</v>
       </c>
-      <c r="L35" s="23">
+      <c r="L35" s="18">
         <v>0.72786778963234999</v>
       </c>
       <c r="M35" s="9">
-        <f>F35*H35/(J35*H35*480*L35)</f>
-        <v>10.500990988951457</v>
+        <f t="shared" si="0"/>
+        <v>9.9880773427401337</v>
       </c>
       <c r="N35" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.579586126886811E-3</v>
       </c>
     </row>
@@ -1435,27 +1459,27 @@
         <v>12407600</v>
       </c>
       <c r="F36">
-        <v>3671000</v>
+        <v>2318000</v>
       </c>
       <c r="G36">
         <v>1000</v>
       </c>
-      <c r="H36" s="25">
+      <c r="H36" s="20">
         <f>2.15905238196507/1000</f>
         <v>2.1590523819650701E-3</v>
       </c>
-      <c r="J36" s="24">
+      <c r="J36" s="19">
         <v>660</v>
       </c>
-      <c r="L36" s="23">
+      <c r="L36" s="18">
         <v>0.69721304997938505</v>
       </c>
       <c r="M36" s="9">
-        <f>F36*H36/(J36*H36*480*L36)</f>
-        <v>16.620102744197272</v>
+        <f t="shared" si="0"/>
+        <v>10.494524151743196</v>
       </c>
       <c r="N36" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5274047246519396E-3</v>
       </c>
     </row>
@@ -1472,22 +1496,22 @@
       <c r="G37">
         <v>1000</v>
       </c>
-      <c r="H37" s="25">
+      <c r="H37" s="20">
         <f>0.66846345040472/1000</f>
         <v>6.6846345040472003E-4</v>
       </c>
-      <c r="J37" s="24">
+      <c r="J37" s="19">
         <v>633.826975537767</v>
       </c>
-      <c r="L37" s="23">
+      <c r="L37" s="18">
         <v>0.82250949258375305</v>
       </c>
       <c r="M37" s="9">
-        <f>F37*H37/(J37*H37*480*L37)</f>
+        <f t="shared" si="0"/>
         <v>0.21979095424129719</v>
       </c>
       <c r="N37" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.9961991680235853E-3</v>
       </c>
     </row>
@@ -1504,22 +1528,22 @@
       <c r="G38">
         <v>1000</v>
       </c>
-      <c r="H38" s="25">
+      <c r="H38" s="20">
         <f>4.45269698507593/1000</f>
         <v>4.4526969850759296E-3</v>
       </c>
-      <c r="J38" s="24">
+      <c r="J38" s="19">
         <v>479.17350733281802</v>
       </c>
-      <c r="L38" s="23">
+      <c r="L38" s="18">
         <v>0.74978989337439095</v>
       </c>
       <c r="M38" s="9">
-        <f>F38*H38/(J38*H38*480*L38)</f>
+        <f t="shared" si="0"/>
         <v>5.7986431344907319E-3</v>
       </c>
       <c r="N38" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.7986431344907319E-3</v>
       </c>
     </row>
@@ -1536,22 +1560,22 @@
       <c r="G39">
         <v>1000</v>
       </c>
-      <c r="H39" s="25">
+      <c r="H39" s="20">
         <f>3.69815107657532/1000</f>
         <v>3.6981510765753201E-3</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="19">
         <v>483.00001144409202</v>
       </c>
-      <c r="L39" s="23">
+      <c r="L39" s="18">
         <v>0.891981577941797</v>
       </c>
       <c r="M39" s="9">
-        <f>F39*H39/(J39*H39*480*L39)</f>
+        <f t="shared" si="0"/>
         <v>4.8356597660512181E-3</v>
       </c>
       <c r="N39" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8356597660512181E-3</v>
       </c>
     </row>
@@ -1568,22 +1592,22 @@
       <c r="G40">
         <v>1000</v>
       </c>
-      <c r="H40" s="25">
+      <c r="H40" s="20">
         <f>3.89941847511468/1000</f>
         <v>3.8994184751146798E-3</v>
       </c>
-      <c r="J40" s="24">
+      <c r="J40" s="19">
         <v>483.00001144409202</v>
       </c>
-      <c r="L40" s="23">
+      <c r="L40" s="18">
         <v>0.83073242756994803</v>
       </c>
       <c r="M40" s="9">
-        <f>F40*H40/(J40*H40*480*L40)</f>
+        <f t="shared" si="0"/>
         <v>13.01681678529294</v>
       </c>
       <c r="N40" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1921885860761628E-3</v>
       </c>
     </row>
@@ -1600,18 +1624,18 @@
       <c r="G41">
         <v>1000</v>
       </c>
-      <c r="H41" s="25">
+      <c r="H41" s="20">
         <f>3.78381132159395/1000</f>
         <v>3.78381132159395E-3</v>
       </c>
-      <c r="J41" s="24">
+      <c r="J41" s="19">
         <v>489.17941116760102</v>
       </c>
-      <c r="L41" s="23">
+      <c r="L41" s="18">
         <v>0.67623798704798499</v>
       </c>
       <c r="M41" s="9">
-        <f>F41*H41/(J41*H41*480*L41)</f>
+        <f t="shared" si="0"/>
         <v>6.2978313937329848E-3</v>
       </c>
       <c r="N41" s="9">
@@ -1626,14 +1650,14 @@
       <c r="E42">
         <v>4502244</v>
       </c>
-      <c r="H42" s="25">
+      <c r="H42" s="20">
         <f>1.79833904216144/1000</f>
         <v>1.7983390421614401E-3</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J42" s="19">
         <v>292.09190942222602</v>
       </c>
-      <c r="L42" s="23">
+      <c r="L42" s="18">
         <v>0.48793678480548203</v>
       </c>
       <c r="M42" s="9"/>
@@ -1646,14 +1670,14 @@
       <c r="E43">
         <v>4605108</v>
       </c>
-      <c r="H43" s="25">
+      <c r="H43" s="20">
         <f>3.99685466418631/1000</f>
         <v>3.9968546641863095E-3</v>
       </c>
-      <c r="J43" s="24">
+      <c r="J43" s="19">
         <v>286.41874550067899</v>
       </c>
-      <c r="L43" s="23">
+      <c r="L43" s="18">
         <v>0.57933407298994299</v>
       </c>
       <c r="M43" s="9"/>
@@ -1666,14 +1690,14 @@
       <c r="E44">
         <v>4888464</v>
       </c>
-      <c r="H44" s="25">
+      <c r="H44" s="20">
         <f>2.98636386831565/1000</f>
         <v>2.98636386831565E-3</v>
       </c>
-      <c r="J44" s="24">
+      <c r="J44" s="19">
         <v>300</v>
       </c>
-      <c r="L44" s="23">
+      <c r="L44" s="18">
         <v>0.64726151267721199</v>
       </c>
       <c r="M44" s="9"/>
@@ -1686,14 +1710,14 @@
       <c r="E45">
         <v>5565444</v>
       </c>
-      <c r="H45" s="25">
+      <c r="H45" s="20">
         <f>2.85934264011567/1000</f>
         <v>2.8593426401156701E-3</v>
       </c>
-      <c r="J45" s="24">
+      <c r="J45" s="19">
         <v>312.85597082724303</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="18">
         <v>0.66834057024015203</v>
       </c>
       <c r="M45" s="9"/>
@@ -1706,14 +1730,14 @@
       <c r="E46">
         <v>3931000</v>
       </c>
-      <c r="H46" s="25">
+      <c r="H46" s="20">
         <f>4.00765759075619/1000</f>
         <v>4.00765759075619E-3</v>
       </c>
-      <c r="J46" s="24">
+      <c r="J46" s="19">
         <v>263.16579583595001</v>
       </c>
-      <c r="L46" s="23">
+      <c r="L46" s="18">
         <v>0.49372229488084601</v>
       </c>
       <c r="M46" s="9"/>
@@ -1726,14 +1750,14 @@
       <c r="E47">
         <v>4196322</v>
       </c>
-      <c r="H47" s="25">
+      <c r="H47" s="20">
         <f>4.37136935664059/1000</f>
         <v>4.3713693566405894E-3</v>
       </c>
-      <c r="J47" s="24">
+      <c r="J47" s="19">
         <v>279.99999046325701</v>
       </c>
-      <c r="L47" s="23">
+      <c r="L47" s="18">
         <v>0.57930844113381696</v>
       </c>
       <c r="M47" s="9"/>
@@ -1746,14 +1770,14 @@
       <c r="E48">
         <v>5157352</v>
       </c>
-      <c r="H48" s="25">
+      <c r="H48" s="20">
         <f>3.1836603956552/1000</f>
         <v>3.1836603956552001E-3</v>
       </c>
-      <c r="J48" s="24">
+      <c r="J48" s="19">
         <v>284.72995178137899</v>
       </c>
-      <c r="L48" s="23">
+      <c r="L48" s="18">
         <v>0.66998113108977297</v>
       </c>
       <c r="M48" s="9"/>
@@ -1766,14 +1790,14 @@
       <c r="E49">
         <v>2632713</v>
       </c>
-      <c r="H49" s="25">
+      <c r="H49" s="20">
         <f>8.93216269229009/1000</f>
         <v>8.9321626922900903E-3</v>
       </c>
-      <c r="J49" s="24">
+      <c r="J49" s="19">
         <v>150.50029379138101</v>
       </c>
-      <c r="L49" s="23">
+      <c r="L49" s="18">
         <v>0.68915148180501296</v>
       </c>
       <c r="M49" s="9"/>
@@ -1786,14 +1810,14 @@
       <c r="E50">
         <v>2005412</v>
       </c>
-      <c r="H50" s="25">
+      <c r="H50" s="20">
         <f>10.1964611046349/1000</f>
         <v>1.0196461104634898E-2</v>
       </c>
-      <c r="J50" s="24">
+      <c r="J50" s="19">
         <v>146.40475074882301</v>
       </c>
-      <c r="L50" s="23">
+      <c r="L50" s="18">
         <v>0.52990503974713299</v>
       </c>
       <c r="M50" s="9"/>
@@ -1806,14 +1830,14 @@
       <c r="E51">
         <v>7251312</v>
       </c>
-      <c r="H51" s="25">
+      <c r="H51" s="20">
         <f>2.33542107577583/1000</f>
         <v>2.3354210757758299E-3</v>
       </c>
-      <c r="J51" s="24">
+      <c r="J51" s="19">
         <v>279.99999046325701</v>
       </c>
-      <c r="L51" s="23">
+      <c r="L51" s="18">
         <v>0.75486486993963497</v>
       </c>
       <c r="M51" s="9"/>
@@ -1826,14 +1850,14 @@
       <c r="E52">
         <v>6086916</v>
       </c>
-      <c r="H52" s="25">
+      <c r="H52" s="20">
         <f>3.24181305143847/1000</f>
         <v>3.2418130514384699E-3</v>
       </c>
-      <c r="J52" s="24">
+      <c r="J52" s="19">
         <v>274.87825511216801</v>
       </c>
-      <c r="L52" s="23">
+      <c r="L52" s="18">
         <v>0.68936781111033496</v>
       </c>
       <c r="M52" s="9"/>
@@ -1846,14 +1870,14 @@
       <c r="E53">
         <v>4209796</v>
       </c>
-      <c r="H53" s="25">
+      <c r="H53" s="20">
         <f>1.8650088585347/1000</f>
         <v>1.8650088585347E-3</v>
       </c>
-      <c r="J53" s="24">
+      <c r="J53" s="19">
         <v>264.09920060626303</v>
       </c>
-      <c r="L53" s="23">
+      <c r="L53" s="18">
         <v>0.54235818587372897</v>
       </c>
       <c r="M53" s="9"/>
@@ -1866,14 +1890,14 @@
       <c r="E54">
         <v>4605340</v>
       </c>
-      <c r="H54" s="25">
+      <c r="H54" s="20">
         <f>2.04443472676232/1000</f>
         <v>2.04443472676232E-3</v>
       </c>
-      <c r="J54" s="24">
+      <c r="J54" s="19">
         <v>284.73175807738698</v>
       </c>
-      <c r="L54" s="23">
+      <c r="L54" s="18">
         <v>0.56223781896990799</v>
       </c>
       <c r="M54" s="9"/>
@@ -1886,14 +1910,14 @@
       <c r="E55">
         <v>4438288</v>
       </c>
-      <c r="H55" s="25">
+      <c r="H55" s="20">
         <f>4.90999985408869/1000</f>
         <v>4.9099998540886904E-3</v>
       </c>
-      <c r="J55" s="24">
+      <c r="J55" s="19">
         <v>260.00000953674299</v>
       </c>
-      <c r="L55" s="23">
+      <c r="L55" s="18">
         <v>0.56317894721065598</v>
       </c>
       <c r="M55" s="9"/>
@@ -1906,14 +1930,14 @@
       <c r="E56">
         <v>1520167</v>
       </c>
-      <c r="H56" s="25">
+      <c r="H56" s="20">
         <f>25.8720012610716/1000</f>
         <v>2.58720012610716E-2</v>
       </c>
-      <c r="J56" s="24">
+      <c r="J56" s="19">
         <v>92.830658335881296</v>
       </c>
-      <c r="L56" s="23">
+      <c r="L56" s="18">
         <v>0.55287646564834803</v>
       </c>
       <c r="M56" s="9"/>
@@ -1926,14 +1950,14 @@
       <c r="E57">
         <v>3040836</v>
       </c>
-      <c r="H57" s="25">
+      <c r="H57" s="20">
         <f>3.92250190209233/1000</f>
         <v>3.9225019020923298E-3</v>
       </c>
-      <c r="J57" s="24">
+      <c r="J57" s="19">
         <v>299.84565678211101</v>
       </c>
-      <c r="L57" s="23">
+      <c r="L57" s="18">
         <v>0.62207607852207103</v>
       </c>
       <c r="M57" s="9"/>
@@ -1946,14 +1970,14 @@
       <c r="E58">
         <v>914952</v>
       </c>
-      <c r="H58" s="25">
+      <c r="H58" s="20">
         <f>26.1312100197428/1000</f>
         <v>2.61312100197428E-2</v>
       </c>
-      <c r="J58" s="24">
+      <c r="J58" s="19">
         <v>87.513553970476096</v>
       </c>
-      <c r="L58" s="23">
+      <c r="L58" s="18">
         <v>0.31301547333277502</v>
       </c>
       <c r="M58" s="9"/>
@@ -1966,14 +1990,14 @@
       <c r="E59">
         <v>619432</v>
       </c>
-      <c r="H59" s="25">
+      <c r="H59" s="20">
         <f>62.3202702976991/1000</f>
         <v>6.2320270297699105E-2</v>
       </c>
-      <c r="J59" s="24">
+      <c r="J59" s="19">
         <v>60.480449534168301</v>
       </c>
-      <c r="L59" s="23">
+      <c r="L59" s="18">
         <v>0.41502337592158201</v>
       </c>
       <c r="M59" s="9"/>
@@ -1986,14 +2010,14 @@
       <c r="E60">
         <v>5507668</v>
       </c>
-      <c r="H60" s="25">
+      <c r="H60" s="20">
         <f>4.99769163699139/1000</f>
         <v>4.9976916369913896E-3</v>
       </c>
-      <c r="J60" s="24">
+      <c r="J60" s="19">
         <v>279.99999046325701</v>
       </c>
-      <c r="L60" s="23">
+      <c r="L60" s="18">
         <v>0.67152074294702602</v>
       </c>
       <c r="M60" s="9"/>
@@ -2006,14 +2030,14 @@
       <c r="E61">
         <v>6828400</v>
       </c>
-      <c r="H61" s="25">
+      <c r="H61" s="20">
         <f>4.68241980228823/1000</f>
         <v>4.6824198022882299E-3</v>
       </c>
-      <c r="J61" s="24">
+      <c r="J61" s="19">
         <v>260.00000953674299</v>
       </c>
-      <c r="L61" s="23">
+      <c r="L61" s="18">
         <v>0.73077789643872104</v>
       </c>
       <c r="M61" s="9"/>
@@ -2026,14 +2050,14 @@
       <c r="E62">
         <v>5567112</v>
       </c>
-      <c r="H62" s="25">
+      <c r="H62" s="20">
         <f>3.95233314877769/1000</f>
         <v>3.9523331487776904E-3</v>
       </c>
-      <c r="J62" s="24">
+      <c r="J62" s="19">
         <v>277.82067109152899</v>
       </c>
-      <c r="L62" s="23">
+      <c r="L62" s="18">
         <v>0.62285858762021695</v>
       </c>
       <c r="M62" s="9"/>
@@ -2046,14 +2070,14 @@
       <c r="E63">
         <v>3268978</v>
       </c>
-      <c r="H63" s="25">
+      <c r="H63" s="20">
         <f>6.93669468434003/1000</f>
         <v>6.9366946843400301E-3</v>
       </c>
-      <c r="J63" s="24">
+      <c r="J63" s="19">
         <v>176.52903509502201</v>
       </c>
-      <c r="L63" s="23">
+      <c r="L63" s="18">
         <v>0.59053560942063699</v>
       </c>
       <c r="M63" s="9"/>
@@ -2066,14 +2090,14 @@
       <c r="E64">
         <v>2206532</v>
       </c>
-      <c r="H64" s="25">
+      <c r="H64" s="20">
         <f>15.5647624267794/1000</f>
         <v>1.5564762426779399E-2</v>
       </c>
-      <c r="J64" s="24">
+      <c r="J64" s="19">
         <v>97.6573178133619</v>
       </c>
-      <c r="L64" s="23">
+      <c r="L64" s="18">
         <v>0.75032931483717602</v>
       </c>
       <c r="M64" s="9"/>
@@ -2086,14 +2110,14 @@
       <c r="E65">
         <v>2358173</v>
       </c>
-      <c r="H65" s="25">
+      <c r="H65" s="20">
         <f>21.7001264386141/1000</f>
         <v>2.17001264386141E-2</v>
       </c>
-      <c r="J65" s="24">
+      <c r="J65" s="19">
         <v>98.674181058758094</v>
       </c>
-      <c r="L65" s="23">
+      <c r="L65" s="18">
         <v>0.74878745231924404</v>
       </c>
       <c r="M65" s="9"/>
@@ -2103,27 +2127,27 @@
       <c r="D66" t="s">
         <v>62</v>
       </c>
-      <c r="E66" s="21">
+      <c r="E66" s="16">
         <f>114985.40625/H66</f>
         <v>34246634.877882801</v>
       </c>
       <c r="F66">
-        <v>7523000</v>
-      </c>
-      <c r="H66" s="25">
+        <v>6100000</v>
+      </c>
+      <c r="H66" s="20">
         <f>3.35756802558899/1000</f>
         <v>3.3575680255889901E-3</v>
       </c>
-      <c r="J66" s="24">
+      <c r="J66" s="19">
         <f>2.57500000298023*(500/H66)</f>
         <v>383462.07483443606</v>
       </c>
-      <c r="L66" s="23">
+      <c r="L66" s="18">
         <v>1.1790338355157499</v>
       </c>
       <c r="M66" s="9">
         <f>F66*H66/(J66*H66*480*L66)</f>
-        <v>3.4665792898722972E-2</v>
+        <v>2.8108645046153145E-2</v>
       </c>
       <c r="N66" s="9"/>
     </row>
@@ -2131,22 +2155,22 @@
       <c r="D67" t="s">
         <v>63</v>
       </c>
-      <c r="E67" s="22">
+      <c r="E67" s="17">
         <f>90653.4375/H67</f>
         <v>1711510.3729148097</v>
       </c>
       <c r="F67">
         <v>57000</v>
       </c>
-      <c r="H67" s="25">
+      <c r="H67" s="20">
         <f>52.9669226284685/1000</f>
         <v>5.2966922628468499E-2</v>
       </c>
-      <c r="J67" s="24">
+      <c r="J67" s="19">
         <f>3.29999998211861*(500/H67)</f>
         <v>31151.517006813381</v>
       </c>
-      <c r="L67" s="23">
+      <c r="L67" s="18">
         <v>0.75279795798154303</v>
       </c>
       <c r="M67" s="9">
@@ -2159,29 +2183,63 @@
       <c r="D68" t="s">
         <v>64</v>
       </c>
-      <c r="E68" s="21">
+      <c r="E68" s="16">
         <f>108075.75/H68</f>
         <v>31899571.911138851</v>
       </c>
       <c r="F68">
-        <v>7523000</v>
-      </c>
-      <c r="H68" s="25">
+        <v>7259000</v>
+      </c>
+      <c r="H68" s="20">
         <f>3.38800001144409/1000</f>
         <v>3.38800001144409E-3</v>
       </c>
-      <c r="J68" s="24">
+      <c r="J68" s="19">
         <f>3.87096762657166*(500/H68)</f>
         <v>571276.2121452461</v>
       </c>
-      <c r="L68" s="23">
+      <c r="L68" s="18">
         <v>0.76389627203334698</v>
       </c>
       <c r="M68" s="9">
         <f>F68*H68/(J68*H68*480*L68)</f>
-        <v>3.5914456070995963E-2</v>
+        <v>3.4654132210469181E-2</v>
       </c>
       <c r="N68" s="9"/>
+    </row>
+    <row r="70" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H70" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J70" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L70" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M70" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>6000000</v>
+      </c>
+      <c r="H71" s="20">
+        <f>AVERAGE(H25:H68)</f>
+        <v>9.3498181599797545E-3</v>
+      </c>
+      <c r="J71" s="19">
+        <f>AVERAGE(J25:J68)</f>
+        <v>22686.65032195509</v>
+      </c>
+      <c r="L71" s="18">
+        <v>1</v>
+      </c>
+      <c r="M71" s="18">
+        <f>F71*H71/(J71*H71*480*L71)</f>
+        <v>0.55098482246641223</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2195,7 +2253,7 @@
     <mergeCell ref="I4:I6"/>
     <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="L25:L68">
+  <conditionalFormatting sqref="L25:L68 L71">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.4"/>

</xml_diff>